<commit_message>
Fixing All JLN Script
</commit_message>
<xml_diff>
--- a/Excel/Excel_Config.xlsx
+++ b/Excel/Excel_Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\Bitvice\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\ICONS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE54D9B-D677-4883-AF50-84FEAFE48895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6F0457-F7A0-4AF8-A52D-B5AA11278B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{6FC7654C-3A1B-4451-AA94-4524C316DE43}"/>
+    <workbookView xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{6FC7654C-3A1B-4451-AA94-4524C316DE43}"/>
   </bookViews>
   <sheets>
     <sheet name="API_CONFIG" sheetId="4" r:id="rId1"/>
@@ -364,9 +364,6 @@
     <t>KSEI</t>
   </si>
   <si>
-    <t>23520</t>
-  </si>
-  <si>
     <t>LOG_FNSTPCA_IP_ADDRESS</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>LOG_FNSONLAD_PASSWORD</t>
+  </si>
+  <si>
+    <t>25154</t>
   </si>
 </sst>
 </file>
@@ -939,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CBBB2C-9A46-4D76-9E03-ECD80CF1429E}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -988,54 +988,54 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
       <c r="F1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" t="s">
         <v>113</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>114</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>115</v>
-      </c>
-      <c r="I1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2">
         <v>22</v>
       </c>
       <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
         <v>110</v>
       </c>
-      <c r="D2" t="s">
-        <v>111</v>
-      </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G2">
         <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1265,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C742778C-BE15-4EF8-AABB-34470A567310}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1311,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Creating Screen 1032 and Fixing
</commit_message>
<xml_diff>
--- a/Excel/Excel_Config.xlsx
+++ b/Excel/Excel_Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\ICONS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6F0457-F7A0-4AF8-A52D-B5AA11278B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A58371-36C4-4998-8A0D-A416ED96373B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{6FC7654C-3A1B-4451-AA94-4524C316DE43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{6FC7654C-3A1B-4451-AA94-4524C316DE43}"/>
   </bookViews>
   <sheets>
     <sheet name="API_CONFIG" sheetId="4" r:id="rId1"/>
@@ -400,7 +400,7 @@
     <t>LOG_FNSONLAD_PASSWORD</t>
   </si>
   <si>
-    <t>25154</t>
+    <t>28594</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>